<commit_message>
fix main y ficheros excel
</commit_message>
<xml_diff>
--- a/resumen_experimentos.xlsx
+++ b/resumen_experimentos.xlsx
@@ -693,28 +693,28 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>3800</v>
+        <v>3798</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>2.4968</v>
+        <v>2.5195</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>33754</v>
+        <v>34112</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>2.8481</v>
+        <v>2.7118</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>13728</v>
+        <v>13718</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>4.6889</v>
+        <v>4.4769</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>190160</v>
+        <v>189834</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>4.7031</v>
+        <v>4.886</v>
       </c>
       <c r="J7" s="2" t="inlineStr">
         <is>
@@ -729,28 +729,28 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>3758</v>
+        <v>3804</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>2.3806</v>
+        <v>2.5768</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>33886</v>
+        <v>34148</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>3.2275</v>
+        <v>2.738</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>13676</v>
+        <v>13692</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>5.2585</v>
+        <v>4.4125</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>190360</v>
+        <v>190080</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>5.0724</v>
+        <v>4.8752</v>
       </c>
       <c r="J8" s="2" t="inlineStr">
         <is>
@@ -765,28 +765,28 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>3760</v>
+        <v>3758</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>2.4625</v>
+        <v>2.5812</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>33268</v>
+        <v>34062</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>2.7686</v>
+        <v>2.7305</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>13708</v>
+        <v>13710</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>4.3584</v>
+        <v>4.3188</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>188464</v>
+        <v>186150</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>4.8233</v>
+        <v>4.7694</v>
       </c>
       <c r="J9" s="2" t="inlineStr">
         <is>
@@ -801,28 +801,28 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>3804</v>
+        <v>3808</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>2.5605</v>
+        <v>2.6448</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>34356</v>
+        <v>34128</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>2.6518</v>
+        <v>2.796</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>13716</v>
+        <v>13708</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>4.8357</v>
+        <v>4.2938</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>189208</v>
+        <v>190480</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>4.7819</v>
+        <v>4.758</v>
       </c>
       <c r="J10" s="2" t="inlineStr">
         <is>
@@ -837,28 +837,28 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>3764</v>
+        <v>3732</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>2.6131</v>
+        <v>2.6433</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>33844</v>
+        <v>33886</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>3.0231</v>
+        <v>2.6869</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>13656</v>
+        <v>13692</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>4.6743</v>
+        <v>4.2632</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>190176</v>
+        <v>189854</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>4.6257</v>
+        <v>4.854</v>
       </c>
       <c r="J11" s="2" t="inlineStr">
         <is>
@@ -873,19 +873,19 @@
         </is>
       </c>
       <c r="B12" s="8" t="n">
-        <v>0.006433077523941778</v>
+        <v>0.00944000762128768</v>
       </c>
       <c r="C12" s="2" t="inlineStr"/>
       <c r="D12" s="8" t="n">
-        <v>0.01442587011470198</v>
+        <v>0.003950562833036846</v>
       </c>
       <c r="E12" s="2" t="inlineStr"/>
       <c r="F12" s="8" t="n">
-        <v>0.002245935378518844</v>
+        <v>0.0008708875190182243</v>
       </c>
       <c r="G12" s="2" t="inlineStr"/>
       <c r="H12" s="8" t="n">
-        <v>0.005397080398868141</v>
+        <v>0.01175001682766531</v>
       </c>
       <c r="I12" s="2" t="inlineStr"/>
       <c r="J12" s="2" t="inlineStr"/>
@@ -897,19 +897,19 @@
         </is>
       </c>
       <c r="B13" s="9" t="n">
-        <v>0.06640316205533597</v>
+        <v>0.06719367588932806</v>
       </c>
       <c r="C13" s="2" t="inlineStr"/>
       <c r="D13" s="9" t="n">
-        <v>0.2584313141836583</v>
+        <v>0.26756957880637</v>
       </c>
       <c r="E13" s="2" t="inlineStr"/>
       <c r="F13" s="9" t="n">
-        <v>0.03045440866686729</v>
+        <v>0.03099608787240446</v>
       </c>
       <c r="G13" s="2" t="inlineStr"/>
       <c r="H13" s="9" t="n">
-        <v>0.2600552721088435</v>
+        <v>0.257437818877551</v>
       </c>
       <c r="I13" s="2" t="inlineStr"/>
       <c r="J13" s="2" t="inlineStr"/>
@@ -1130,28 +1130,28 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>3634</v>
+        <v>3614</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>2.5096</v>
+        <v>2.6167</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>31230</v>
+        <v>30824</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>2.8356</v>
+        <v>2.7784</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>13366</v>
+        <v>13362</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>4.3321</v>
+        <v>6.4688</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>176470</v>
+        <v>176198</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>4.7123</v>
+        <v>4.8272</v>
       </c>
       <c r="J7" s="2" t="inlineStr">
         <is>
@@ -1166,28 +1166,28 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>3654</v>
+        <v>3630</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>2.5259</v>
+        <v>2.6236</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>31352</v>
+        <v>31092</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>2.6867</v>
+        <v>2.8552</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>13396</v>
+        <v>13352</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>4.3369</v>
+        <v>4.5663</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>175590</v>
+        <v>174432</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>4.6912</v>
+        <v>4.8448</v>
       </c>
       <c r="J8" s="2" t="inlineStr">
         <is>
@@ -1202,28 +1202,28 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>3636</v>
+        <v>3640</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>2.5924</v>
+        <v>2.6783</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>30950</v>
+        <v>31120</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>2.5703</v>
+        <v>2.7964</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>13386</v>
+        <v>13420</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>4.2727</v>
+        <v>4.478</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>174212</v>
+        <v>174368</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>4.7137</v>
+        <v>4.9082</v>
       </c>
       <c r="J9" s="2" t="inlineStr">
         <is>
@@ -1238,28 +1238,28 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>3638</v>
+        <v>3654</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>2.5588</v>
+        <v>2.7032</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>30566</v>
+        <v>31558</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>2.7078</v>
+        <v>2.8012</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>13360</v>
+        <v>13358</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>4.252</v>
+        <v>4.3144</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>176080</v>
+        <v>150528</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>4.6952</v>
+        <v>4.8264</v>
       </c>
       <c r="J10" s="2" t="inlineStr">
         <is>
@@ -1274,28 +1274,28 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>3648</v>
+        <v>3650</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>2.5634</v>
+        <v>2.6177</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>31580</v>
+        <v>31310</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>2.5691</v>
+        <v>2.817</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>13362</v>
+        <v>13348</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>4.3023</v>
+        <v>4.4288</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>174698</v>
+        <v>150528</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>4.704</v>
+        <v>4.7734</v>
       </c>
       <c r="J11" s="2" t="inlineStr">
         <is>
@@ -1310,19 +1310,19 @@
         </is>
       </c>
       <c r="B12" s="8" t="n">
-        <v>0.002428663260034619</v>
+        <v>0.004559374192701604</v>
       </c>
       <c r="C12" s="2" t="inlineStr"/>
       <c r="D12" s="8" t="n">
-        <v>0.01455542168478851</v>
+        <v>0.0101534129024161</v>
       </c>
       <c r="E12" s="2" t="inlineStr"/>
       <c r="F12" s="8" t="n">
-        <v>0.001208424496254064</v>
+        <v>0.002224156710667241</v>
       </c>
       <c r="G12" s="2" t="inlineStr"/>
       <c r="H12" s="8" t="n">
-        <v>0.006255848831307265</v>
+        <v>0.08917679470380416</v>
       </c>
       <c r="I12" s="2" t="inlineStr"/>
       <c r="J12" s="2" t="inlineStr"/>
@@ -1334,19 +1334,19 @@
         </is>
       </c>
       <c r="B13" s="9" t="n">
-        <v>0.0282326369282891</v>
+        <v>0.02699040090344438</v>
       </c>
       <c r="C13" s="2" t="inlineStr"/>
       <c r="D13" s="9" t="n">
-        <v>0.1584908468522102</v>
+        <v>0.1601726447388004</v>
       </c>
       <c r="E13" s="2" t="inlineStr"/>
       <c r="F13" s="9" t="n">
-        <v>0.006169124285284382</v>
+        <v>0.005717724947336744</v>
       </c>
       <c r="G13" s="2" t="inlineStr"/>
       <c r="H13" s="9" t="n">
-        <v>0.1652981505102041</v>
+        <v>0.09754198554421768</v>
       </c>
       <c r="I13" s="2" t="inlineStr"/>
       <c r="J13" s="2" t="inlineStr"/>
@@ -1567,28 +1567,28 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>3770</v>
+        <v>3806</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>2.7531</v>
+        <v>2.6094</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>33974</v>
+        <v>33770</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>3.021</v>
+        <v>2.7478</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>13676</v>
+        <v>13684</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>4.4759</v>
+        <v>4.6529</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>190830</v>
+        <v>190212</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>4.8639</v>
+        <v>4.8995</v>
       </c>
       <c r="J7" s="2" t="inlineStr">
         <is>
@@ -1603,28 +1603,28 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>3766</v>
+        <v>3788</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>2.6853</v>
+        <v>2.5277</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>33790</v>
+        <v>33966</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>2.8678</v>
+        <v>2.8006</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>13704</v>
+        <v>13706</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>5.4541</v>
+        <v>4.4462</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>190660</v>
+        <v>190138</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>4.9003</v>
+        <v>4.8664</v>
       </c>
       <c r="J8" s="2" t="inlineStr">
         <is>
@@ -1639,28 +1639,28 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>3780</v>
+        <v>3786</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>2.673</v>
+        <v>2.5051</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>33566</v>
+        <v>33178</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>2.9605</v>
+        <v>2.7474</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>13702</v>
+        <v>13722</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>4.4526</v>
+        <v>4.4021</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>188754</v>
+        <v>191124</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>5.0852</v>
+        <v>4.8798</v>
       </c>
       <c r="J9" s="2" t="inlineStr">
         <is>
@@ -1675,28 +1675,28 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>3792</v>
+        <v>3790</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>2.8172</v>
+        <v>2.6444</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>33656</v>
+        <v>33918</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>2.9367</v>
+        <v>2.7319</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>13718</v>
+        <v>13666</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>5.7914</v>
+        <v>4.3792</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>190418</v>
+        <v>189576</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>5.1644</v>
+        <v>4.8943</v>
       </c>
       <c r="J10" s="2" t="inlineStr">
         <is>
@@ -1711,28 +1711,28 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>3818</v>
+        <v>3790</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>2.653</v>
+        <v>2.6562</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>33618</v>
+        <v>34000</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>2.9524</v>
+        <v>2.7263</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>13690</v>
+        <v>13632</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>4.4859</v>
+        <v>4.326</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>189362</v>
+        <v>190826</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>4.7794</v>
+        <v>4.9711</v>
       </c>
       <c r="J11" s="2" t="inlineStr">
         <is>
@@ -1747,19 +1747,19 @@
         </is>
       </c>
       <c r="B12" s="8" t="n">
-        <v>0.005903254675860023</v>
+        <v>0.00225861095426313</v>
       </c>
       <c r="C12" s="2" t="inlineStr"/>
       <c r="D12" s="8" t="n">
-        <v>0.006103368908595369</v>
+        <v>0.01266735899017488</v>
       </c>
       <c r="E12" s="2" t="inlineStr"/>
       <c r="F12" s="8" t="n">
-        <v>0.001189541701838844</v>
+        <v>0.002642817946170674</v>
       </c>
       <c r="G12" s="2" t="inlineStr"/>
       <c r="H12" s="8" t="n">
-        <v>0.005996154632828841</v>
+        <v>0.004048508029817847</v>
       </c>
       <c r="I12" s="2" t="inlineStr"/>
       <c r="J12" s="2" t="inlineStr"/>
@@ -1771,19 +1771,19 @@
         </is>
       </c>
       <c r="B13" s="9" t="n">
-        <v>0.06866177300959909</v>
+        <v>0.07058159232072275</v>
       </c>
       <c r="C13" s="2" t="inlineStr"/>
       <c r="D13" s="9" t="n">
-        <v>0.2546807560648906</v>
+        <v>0.2563774371186188</v>
       </c>
       <c r="E13" s="2" t="inlineStr"/>
       <c r="F13" s="9" t="n">
-        <v>0.03054468853445682</v>
+        <v>0.02934095696659645</v>
       </c>
       <c r="G13" s="2" t="inlineStr"/>
       <c r="H13" s="9" t="n">
-        <v>0.2622555272108844</v>
+        <v>0.2647161989795919</v>
       </c>
       <c r="I13" s="2" t="inlineStr"/>
       <c r="J13" s="2" t="inlineStr"/>
@@ -2004,28 +2004,28 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>3636</v>
+        <v>3614</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>2.6111</v>
+        <v>2.5839</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>26876</v>
+        <v>31020</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>2.6992</v>
+        <v>2.7088</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>13362</v>
+        <v>13384</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>4.0618</v>
+        <v>4.2999</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>177562</v>
+        <v>174566</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>4.599</v>
+        <v>4.7664</v>
       </c>
       <c r="J7" s="2" t="inlineStr">
         <is>
@@ -2040,28 +2040,28 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>3678</v>
+        <v>3622</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>2.5493</v>
+        <v>2.5844</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>31172</v>
+        <v>31094</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>2.5057</v>
+        <v>2.6765</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>13350</v>
+        <v>13480</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>4.1941</v>
+        <v>4.9733</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>177500</v>
+        <v>176556</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>4.6809</v>
+        <v>4.7456</v>
       </c>
       <c r="J8" s="2" t="inlineStr">
         <is>
@@ -2076,28 +2076,28 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>3628</v>
+        <v>3632</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>2.5132</v>
+        <v>2.52</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>30012</v>
+        <v>31310</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>2.5494</v>
+        <v>2.6656</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>13354</v>
+        <v>13342</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>4.165</v>
+        <v>4.2731</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>157068</v>
+        <v>178918</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>4.5219</v>
+        <v>4.78</v>
       </c>
       <c r="J9" s="2" t="inlineStr">
         <is>
@@ -2112,28 +2112,28 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>3606</v>
+        <v>3616</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>2.5256</v>
+        <v>2.465</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>30868</v>
+        <v>31066</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>2.5048</v>
+        <v>2.7263</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>13362</v>
+        <v>13368</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>4.3498</v>
+        <v>4.1854</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>175606</v>
+        <v>174978</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>4.5935</v>
+        <v>4.7185</v>
       </c>
       <c r="J10" s="2" t="inlineStr">
         <is>
@@ -2148,28 +2148,28 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>3620</v>
+        <v>3672</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>2.4847</v>
+        <v>2.5266</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>31184</v>
+        <v>31690</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>2.5562</v>
+        <v>2.6764</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>13362</v>
+        <v>13542</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>4.1372</v>
+        <v>4.437</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>176696</v>
+        <v>174752</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>4.5756</v>
+        <v>4.781</v>
       </c>
       <c r="J11" s="2" t="inlineStr">
         <is>
@@ -2184,19 +2184,19 @@
         </is>
       </c>
       <c r="B12" s="8" t="n">
-        <v>0.007673877930477455</v>
+        <v>0.006735717880721242</v>
       </c>
       <c r="C12" s="2" t="inlineStr"/>
       <c r="D12" s="8" t="n">
-        <v>0.06781104798417237</v>
+        <v>0.01031324016802704</v>
       </c>
       <c r="E12" s="2" t="inlineStr"/>
       <c r="F12" s="8" t="n">
-        <v>0.0004255833771811902</v>
+        <v>0.006352286342784302</v>
       </c>
       <c r="G12" s="2" t="inlineStr"/>
       <c r="H12" s="8" t="n">
-        <v>0.0589792529826285</v>
+        <v>0.01219165569994979</v>
       </c>
       <c r="I12" s="2" t="inlineStr"/>
       <c r="J12" s="2" t="inlineStr"/>
@@ -2208,19 +2208,19 @@
         </is>
       </c>
       <c r="B13" s="9" t="n">
-        <v>0.02586109542631282</v>
+        <v>0.02518351214003388</v>
       </c>
       <c r="C13" s="2" t="inlineStr"/>
       <c r="D13" s="9" t="n">
-        <v>0.1170709927072481</v>
+        <v>0.1622265218038399</v>
       </c>
       <c r="E13" s="2" t="inlineStr"/>
       <c r="F13" s="9" t="n">
-        <v>0.004965392717424015</v>
+        <v>0.009870598856455011</v>
       </c>
       <c r="G13" s="2" t="inlineStr"/>
       <c r="H13" s="9" t="n">
-        <v>0.1485331632653061</v>
+        <v>0.1689120960884354</v>
       </c>
       <c r="I13" s="2" t="inlineStr"/>
       <c r="J13" s="2" t="inlineStr"/>
@@ -2441,28 +2441,28 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>3612</v>
+        <v>3608</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>2.5321</v>
+        <v>2.6557</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>30684</v>
+        <v>30252</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>2.7394</v>
+        <v>2.731</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>13342</v>
+        <v>13350</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>4.2817</v>
+        <v>4.3333</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>176896</v>
+        <v>176660</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>4.6255</v>
+        <v>4.7503</v>
       </c>
       <c r="J7" s="2" t="inlineStr">
         <is>
@@ -2477,28 +2477,28 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>3656</v>
+        <v>3624</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>2.49</v>
+        <v>2.5457</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>31174</v>
+        <v>26876</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>2.5369</v>
+        <v>2.6225</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>13360</v>
+        <v>13374</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>4.2087</v>
+        <v>6.4163</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>175874</v>
+        <v>175770</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>4.6035</v>
+        <v>4.7432</v>
       </c>
       <c r="J8" s="2" t="inlineStr">
         <is>
@@ -2513,28 +2513,28 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>3622</v>
+        <v>3624</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>2.498</v>
+        <v>2.5461</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>31368</v>
+        <v>31042</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>2.5539</v>
+        <v>2.6708</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>13360</v>
+        <v>13366</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>4.1686</v>
+        <v>4.2433</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>177148</v>
+        <v>176794</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>4.5766</v>
+        <v>4.697</v>
       </c>
       <c r="J9" s="2" t="inlineStr">
         <is>
@@ -2549,28 +2549,28 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>3610</v>
+        <v>3658</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>2.4937</v>
+        <v>2.5329</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>31390</v>
+        <v>30690</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>2.6038</v>
+        <v>2.6541</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>13386</v>
+        <v>13406</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>4.2543</v>
+        <v>4.2367</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>176912</v>
+        <v>175164</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>4.5716</v>
+        <v>4.7297</v>
       </c>
       <c r="J10" s="2" t="inlineStr">
         <is>
@@ -2585,28 +2585,28 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>3626</v>
+        <v>3584</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>2.5336</v>
+        <v>2.5203</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>31398</v>
+        <v>31242</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>2.6169</v>
+        <v>2.6991</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>13358</v>
+        <v>13400</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>4.1408</v>
+        <v>4.2745</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>175174</v>
+        <v>176960</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>4.5482</v>
+        <v>4.7248</v>
       </c>
       <c r="J11" s="2" t="inlineStr">
         <is>
@@ -2621,19 +2621,19 @@
         </is>
       </c>
       <c r="B12" s="8" t="n">
-        <v>0.005215019712713187</v>
+        <v>0.007621766245690324</v>
       </c>
       <c r="C12" s="2" t="inlineStr"/>
       <c r="D12" s="8" t="n">
-        <v>0.01132277962138156</v>
+        <v>0.06688434291863454</v>
       </c>
       <c r="E12" s="2" t="inlineStr"/>
       <c r="F12" s="8" t="n">
-        <v>0.001187636910061458</v>
+        <v>0.001766299198414588</v>
       </c>
       <c r="G12" s="2" t="inlineStr"/>
       <c r="H12" s="8" t="n">
-        <v>0.005605029845360693</v>
+        <v>0.005120082451207098</v>
       </c>
       <c r="I12" s="2" t="inlineStr"/>
       <c r="J12" s="2" t="inlineStr"/>
@@ -2645,19 +2645,19 @@
         </is>
       </c>
       <c r="B13" s="9" t="n">
-        <v>0.02348955392433653</v>
+        <v>0.02190852625635234</v>
       </c>
       <c r="C13" s="2" t="inlineStr"/>
       <c r="D13" s="9" t="n">
-        <v>0.1609912189313886</v>
+        <v>0.1169965768715583</v>
       </c>
       <c r="E13" s="2" t="inlineStr"/>
       <c r="F13" s="9" t="n">
-        <v>0.005206139030996088</v>
+        <v>0.006560337044839001</v>
       </c>
       <c r="G13" s="2" t="inlineStr"/>
       <c r="H13" s="9" t="n">
-        <v>0.1718803146258504</v>
+        <v>0.1710087159863946</v>
       </c>
       <c r="I13" s="2" t="inlineStr"/>
       <c r="J13" s="2" t="inlineStr"/>
@@ -2878,28 +2878,28 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>3634</v>
+        <v>3644</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>2.6169</v>
+        <v>2.6002</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>31406</v>
+        <v>30406</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>2.8553</v>
+        <v>2.6957</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>13380</v>
+        <v>13360</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>4.2632</v>
+        <v>6.2711</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>178576</v>
+        <v>177854</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>4.6946</v>
+        <v>4.7504</v>
       </c>
       <c r="J7" s="2" t="inlineStr">
         <is>
@@ -2914,28 +2914,28 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>3624</v>
+        <v>3638</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>2.5185</v>
+        <v>2.5463</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>28380</v>
+        <v>30830</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>2.4996</v>
+        <v>2.6748</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>13374</v>
+        <v>13368</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>4.2412</v>
+        <v>5.6642</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>174694</v>
+        <v>174738</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>4.5703</v>
+        <v>4.7938</v>
       </c>
       <c r="J8" s="2" t="inlineStr">
         <is>
@@ -2950,28 +2950,28 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>3628</v>
+        <v>3598</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>2.5697</v>
+        <v>2.5222</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>31072</v>
+        <v>31076</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>2.7057</v>
+        <v>2.6724</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>13358</v>
+        <v>13326</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>4.253</v>
+        <v>4.2654</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>174962</v>
+        <v>176518</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>4.8148</v>
+        <v>4.7329</v>
       </c>
       <c r="J9" s="2" t="inlineStr">
         <is>
@@ -2986,28 +2986,28 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>3598</v>
+        <v>3650</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>2.4991</v>
+        <v>2.57</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>29676</v>
+        <v>31528</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>2.4877</v>
+        <v>2.6741</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>13370</v>
+        <v>13480</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>4.0987</v>
+        <v>4.3941</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>175226</v>
+        <v>177372</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>4.549</v>
+        <v>4.7626</v>
       </c>
       <c r="J10" s="2" t="inlineStr">
         <is>
@@ -3022,28 +3022,28 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>3640</v>
+        <v>3602</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>2.5056</v>
+        <v>2.5378</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>30758</v>
+        <v>30754</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>2.6086</v>
+        <v>2.7014</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>13402</v>
+        <v>13362</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>4.3589</v>
+        <v>4.2045</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>174874</v>
+        <v>176362</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>4.6018</v>
+        <v>4.8013</v>
       </c>
       <c r="J11" s="2" t="inlineStr">
         <is>
@@ -3058,19 +3058,19 @@
         </is>
       </c>
       <c r="B12" s="8" t="n">
-        <v>0.004562869305666161</v>
+        <v>0.00692016429129465</v>
       </c>
       <c r="C12" s="2" t="inlineStr"/>
       <c r="D12" s="8" t="n">
-        <v>0.04593372538604845</v>
+        <v>0.01549660420012741</v>
       </c>
       <c r="E12" s="2" t="inlineStr"/>
       <c r="F12" s="8" t="n">
-        <v>0.001220541666606876</v>
+        <v>0.004415876172637593</v>
       </c>
       <c r="G12" s="2" t="inlineStr"/>
       <c r="H12" s="8" t="n">
-        <v>0.01088027034119199</v>
+        <v>0.007926165802842482</v>
       </c>
       <c r="I12" s="2" t="inlineStr"/>
       <c r="J12" s="2" t="inlineStr"/>
@@ -3082,19 +3082,19 @@
         </is>
       </c>
       <c r="B13" s="9" t="n">
-        <v>0.02337662337662338</v>
+        <v>0.023828345567476</v>
       </c>
       <c r="C13" s="2" t="inlineStr"/>
       <c r="D13" s="9" t="n">
-        <v>0.1258520613186486</v>
+        <v>0.150424170263432</v>
       </c>
       <c r="E13" s="2" t="inlineStr"/>
       <c r="F13" s="9" t="n">
-        <v>0.006379777309659946</v>
+        <v>0.006560337044839001</v>
       </c>
       <c r="G13" s="2" t="inlineStr"/>
       <c r="H13" s="9" t="n">
-        <v>0.1670014880952381</v>
+        <v>0.1729963860544218</v>
       </c>
       <c r="I13" s="2" t="inlineStr"/>
       <c r="J13" s="2" t="inlineStr"/>
@@ -3315,28 +3315,28 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>3654</v>
+        <v>3636</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>2.452</v>
+        <v>2.63</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>30846</v>
+        <v>30698</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>2.5469</v>
+        <v>2.6822</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>13360</v>
+        <v>13368</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>4.1375</v>
+        <v>5.1427</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>176502</v>
+        <v>174060</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>4.6472</v>
+        <v>4.7705</v>
       </c>
       <c r="J7" s="2" t="inlineStr">
         <is>
@@ -3351,28 +3351,28 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>3620</v>
+        <v>3642</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>2.4892</v>
+        <v>2.5209</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>31510</v>
+        <v>26876</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>2.5342</v>
+        <v>2.6595</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>13382</v>
+        <v>13448</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>4.2111</v>
+        <v>4.3386</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>175640</v>
+        <v>176530</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>4.5852</v>
+        <v>4.8189</v>
       </c>
       <c r="J8" s="2" t="inlineStr">
         <is>
@@ -3387,28 +3387,28 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>3636</v>
+        <v>3616</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>2.5173</v>
+        <v>2.503</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>26876</v>
+        <v>30924</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>2.5141</v>
+        <v>2.7028</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>13336</v>
+        <v>13330</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>4.2028</v>
+        <v>4.2977</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>176558</v>
+        <v>176608</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>4.6099</v>
+        <v>4.7508</v>
       </c>
       <c r="J9" s="2" t="inlineStr">
         <is>
@@ -3423,28 +3423,28 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>3620</v>
+        <v>3654</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>2.538</v>
+        <v>2.5368</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>26876</v>
+        <v>31526</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>2.5584</v>
+        <v>2.7421</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>13356</v>
+        <v>13318</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>4.1651</v>
+        <v>4.3146</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>177020</v>
+        <v>176410</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>4.5523</v>
+        <v>4.6937</v>
       </c>
       <c r="J10" s="2" t="inlineStr">
         <is>
@@ -3459,28 +3459,28 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>3638</v>
+        <v>3626</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>2.5166</v>
+        <v>2.5748</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>26876</v>
+        <v>31012</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>2.5356</v>
+        <v>2.6458</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>13380</v>
+        <v>13388</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>4.1934</v>
+        <v>4.3205</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>177636</v>
+        <v>175970</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>4.5861</v>
+        <v>4.7269</v>
       </c>
       <c r="J11" s="2" t="inlineStr">
         <is>
@@ -3495,19 +3495,19 @@
         </is>
       </c>
       <c r="B12" s="8" t="n">
-        <v>0.004020549546904098</v>
+        <v>0.004122351721839407</v>
       </c>
       <c r="C12" s="2" t="inlineStr"/>
       <c r="D12" s="8" t="n">
-        <v>0.08810716470344192</v>
+        <v>0.07020010277009375</v>
       </c>
       <c r="E12" s="2" t="inlineStr"/>
       <c r="F12" s="8" t="n">
-        <v>0.001425863104481749</v>
+        <v>0.003893855335040625</v>
       </c>
       <c r="G12" s="2" t="inlineStr"/>
       <c r="H12" s="8" t="n">
-        <v>0.004878762485476765</v>
+        <v>0.007083392717887427</v>
       </c>
       <c r="I12" s="2" t="inlineStr"/>
       <c r="J12" s="2" t="inlineStr"/>
@@ -3519,19 +3519,19 @@
         </is>
       </c>
       <c r="B13" s="9" t="n">
-        <v>0.02586109542631282</v>
+        <v>0.02619988706945229</v>
       </c>
       <c r="C13" s="2" t="inlineStr"/>
       <c r="D13" s="9" t="n">
-        <v>0.06402738502753386</v>
+        <v>0.1239470159249888</v>
       </c>
       <c r="E13" s="2" t="inlineStr"/>
       <c r="F13" s="9" t="n">
-        <v>0.005326512187782124</v>
+        <v>0.005898284682515799</v>
       </c>
       <c r="G13" s="2" t="inlineStr"/>
       <c r="H13" s="9" t="n">
-        <v>0.1736766581632653</v>
+        <v>0.1686569940476191</v>
       </c>
       <c r="I13" s="2" t="inlineStr"/>
       <c r="J13" s="2" t="inlineStr"/>
@@ -3752,28 +3752,28 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>3628</v>
+        <v>3596</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>2.6435</v>
+        <v>2.5891</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>31058</v>
+        <v>26876</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>2.9615</v>
+        <v>2.7204</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>13484</v>
+        <v>13526</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>4.3328</v>
+        <v>4.4224</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>184266</v>
+        <v>176442</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>4.8157</v>
+        <v>4.9371</v>
       </c>
       <c r="J7" s="2" t="inlineStr">
         <is>
@@ -3791,25 +3791,25 @@
         <v>3620</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>2.5511</v>
+        <v>2.5751</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>30128</v>
+        <v>26876</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>2.5965</v>
+        <v>2.7085</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>13364</v>
+        <v>13380</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>4.3505</v>
+        <v>5.4836</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>175582</v>
+        <v>184062</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>4.7076</v>
+        <v>4.8819</v>
       </c>
       <c r="J8" s="2" t="inlineStr">
         <is>
@@ -3824,28 +3824,28 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>3690</v>
+        <v>3626</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>2.5615</v>
+        <v>2.6366</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>30972</v>
+        <v>30912</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>2.5845</v>
+        <v>2.81</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>13370</v>
+        <v>13502</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>4.3643</v>
+        <v>4.4215</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>184752</v>
+        <v>178948</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>4.7559</v>
+        <v>4.9611</v>
       </c>
       <c r="J9" s="2" t="inlineStr">
         <is>
@@ -3860,28 +3860,28 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>3666</v>
+        <v>3646</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>2.5246</v>
+        <v>2.6282</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>31048</v>
+        <v>31030</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>2.6193</v>
+        <v>2.8165</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>13376</v>
+        <v>13356</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>4.3828</v>
+        <v>4.4075</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>182846</v>
+        <v>176644</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>4.7542</v>
+        <v>4.8201</v>
       </c>
       <c r="J10" s="2" t="inlineStr">
         <is>
@@ -3896,28 +3896,28 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>3632</v>
+        <v>3644</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>2.5375</v>
+        <v>2.6714</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>31878</v>
+        <v>30672</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>2.6264</v>
+        <v>2.7895</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>13518</v>
+        <v>13348</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>4.2759</v>
+        <v>4.2996</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>176462</v>
+        <v>178226</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>4.7603</v>
+        <v>4.8757</v>
       </c>
       <c r="J11" s="2" t="inlineStr">
         <is>
@@ -3932,19 +3932,19 @@
         </is>
       </c>
       <c r="B12" s="8" t="n">
-        <v>0.008380861957574244</v>
+        <v>0.005750039353179432</v>
       </c>
       <c r="C12" s="2" t="inlineStr"/>
       <c r="D12" s="8" t="n">
-        <v>0.02305922096833261</v>
+        <v>0.08156470550530785</v>
       </c>
       <c r="E12" s="2" t="inlineStr"/>
       <c r="F12" s="8" t="n">
-        <v>0.005482638869144971</v>
+        <v>0.006384991821910953</v>
       </c>
       <c r="G12" s="2" t="inlineStr"/>
       <c r="H12" s="8" t="n">
-        <v>0.02930991221461893</v>
+        <v>0.02053725014346087</v>
       </c>
       <c r="I12" s="2" t="inlineStr"/>
       <c r="J12" s="2" t="inlineStr"/>
@@ -3956,19 +3956,19 @@
         </is>
       </c>
       <c r="B13" s="9" t="n">
-        <v>0.02970073404856013</v>
+        <v>0.023828345567476</v>
       </c>
       <c r="C13" s="2" t="inlineStr"/>
       <c r="D13" s="9" t="n">
-        <v>0.154070546212234</v>
+        <v>0.08919482065783599</v>
       </c>
       <c r="E13" s="2" t="inlineStr"/>
       <c r="F13" s="9" t="n">
-        <v>0.009810412278061991</v>
+        <v>0.009810412278061993</v>
       </c>
       <c r="G13" s="2" t="inlineStr"/>
       <c r="H13" s="9" t="n">
-        <v>0.2009832057823129</v>
+        <v>0.1882467049319728</v>
       </c>
       <c r="I13" s="2" t="inlineStr"/>
       <c r="J13" s="2" t="inlineStr"/>
@@ -4189,28 +4189,28 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>3624</v>
+        <v>3634</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>2.5437</v>
+        <v>2.5672</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>30834</v>
+        <v>26876</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>2.9277</v>
+        <v>2.7549</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>13368</v>
+        <v>13358</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>4.3856</v>
+        <v>4.5358</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>176712</v>
+        <v>175182</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>4.6848</v>
+        <v>4.84</v>
       </c>
       <c r="J7" s="2" t="inlineStr">
         <is>
@@ -4225,28 +4225,28 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>3634</v>
+        <v>3606</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>2.5289</v>
+        <v>2.6415</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>30252</v>
+        <v>30926</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>2.6335</v>
+        <v>2.8308</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>13354</v>
+        <v>13380</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>4.3611</v>
+        <v>6.6262</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>175622</v>
+        <v>176046</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>4.6407</v>
+        <v>4.7922</v>
       </c>
       <c r="J8" s="2" t="inlineStr">
         <is>
@@ -4261,28 +4261,28 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>3626</v>
+        <v>3612</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>2.5311</v>
+        <v>2.6259</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>30980</v>
+        <v>31704</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>2.5559</v>
+        <v>2.7971</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>13360</v>
+        <v>13376</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>4.2053</v>
+        <v>4.4745</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>175348</v>
+        <v>176384</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>4.6864</v>
+        <v>4.8299</v>
       </c>
       <c r="J9" s="2" t="inlineStr">
         <is>
@@ -4297,28 +4297,28 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>3612</v>
+        <v>3620</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>2.6676</v>
+        <v>2.6586</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>26876</v>
+        <v>30560</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>2.7357</v>
+        <v>2.7848</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>13390</v>
+        <v>13346</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>4.6323</v>
+        <v>4.3566</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>173704</v>
+        <v>174886</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>4.7064</v>
+        <v>4.8284</v>
       </c>
       <c r="J10" s="2" t="inlineStr">
         <is>
@@ -4333,28 +4333,28 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>3652</v>
+        <v>3616</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>2.5302</v>
+        <v>2.6547</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>31448</v>
+        <v>31226</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>2.5548</v>
+        <v>2.7777</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>13366</v>
+        <v>13386</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>4.2677</v>
+        <v>4.4291</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>173530</v>
+        <v>176458</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>4.6259</v>
+        <v>4.8493</v>
       </c>
       <c r="J11" s="2" t="inlineStr">
         <is>
@@ -4369,19 +4369,19 @@
         </is>
       </c>
       <c r="B12" s="8" t="n">
-        <v>0.004176140505273991</v>
+        <v>0.002971811940585154</v>
       </c>
       <c r="C12" s="2" t="inlineStr"/>
       <c r="D12" s="8" t="n">
-        <v>0.06846944386557524</v>
+        <v>0.07206072732170327</v>
       </c>
       <c r="E12" s="2" t="inlineStr"/>
       <c r="F12" s="8" t="n">
-        <v>0.001028248544283472</v>
+        <v>0.00125258232851444</v>
       </c>
       <c r="G12" s="2" t="inlineStr"/>
       <c r="H12" s="8" t="n">
-        <v>0.008961069312525308</v>
+        <v>0.00475756982652139</v>
       </c>
       <c r="I12" s="2" t="inlineStr"/>
       <c r="J12" s="2" t="inlineStr"/>
@@ -4393,19 +4393,19 @@
         </is>
       </c>
       <c r="B13" s="9" t="n">
-        <v>0.02473178994918125</v>
+        <v>0.02134387351778656</v>
       </c>
       <c r="C13" s="2" t="inlineStr"/>
       <c r="D13" s="9" t="n">
-        <v>0.1191397529394255</v>
+        <v>0.1258520613186486</v>
       </c>
       <c r="E13" s="2" t="inlineStr"/>
       <c r="F13" s="9" t="n">
-        <v>0.005687631658140234</v>
+        <v>0.005808004814926272</v>
       </c>
       <c r="G13" s="2" t="inlineStr"/>
       <c r="H13" s="9" t="n">
-        <v>0.1624627976190476</v>
+        <v>0.1678305697278911</v>
       </c>
       <c r="I13" s="2" t="inlineStr"/>
       <c r="J13" s="2" t="inlineStr"/>
@@ -4626,28 +4626,28 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>3610</v>
+        <v>3616</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>2.6409</v>
+        <v>2.5929</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>30958</v>
+        <v>30906</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>2.8525</v>
+        <v>2.7595</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>13336</v>
+        <v>13486</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>4.3664</v>
+        <v>5.7754</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>173724</v>
+        <v>176898</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>4.7111</v>
+        <v>4.8451</v>
       </c>
       <c r="J7" s="2" t="inlineStr">
         <is>
@@ -4662,28 +4662,28 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>3662</v>
+        <v>3598</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>2.5331</v>
+        <v>2.6272</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>30668</v>
+        <v>30892</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>2.6604</v>
+        <v>2.7735</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>13374</v>
+        <v>13386</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>4.3195</v>
+        <v>6.8219</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>176212</v>
+        <v>175676</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>4.7862</v>
+        <v>4.8402</v>
       </c>
       <c r="J8" s="2" t="inlineStr">
         <is>
@@ -4698,28 +4698,28 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>3648</v>
+        <v>3620</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>2.5282</v>
+        <v>2.6663</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>30774</v>
+        <v>31298</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>2.5785</v>
+        <v>2.7646</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>13350</v>
+        <v>13370</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>4.3153</v>
+        <v>4.4835</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>175880</v>
+        <v>177638</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>4.6923</v>
+        <v>4.8527</v>
       </c>
       <c r="J9" s="2" t="inlineStr">
         <is>
@@ -4734,28 +4734,28 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>3630</v>
+        <v>3624</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>2.5391</v>
+        <v>2.6277</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>26876</v>
+        <v>29116</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>2.6329</v>
+        <v>2.7904</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>13342</v>
+        <v>13340</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>4.2093</v>
+        <v>4.4485</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>174982</v>
+        <v>175050</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>4.7171</v>
+        <v>4.7965</v>
       </c>
       <c r="J10" s="2" t="inlineStr">
         <is>
@@ -4770,28 +4770,28 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>3646</v>
+        <v>3610</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>2.6413</v>
+        <v>2.7083</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>31164</v>
+        <v>30746</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>2.5833</v>
+        <v>2.8055</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>13472</v>
+        <v>13380</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>4.3053</v>
+        <v>4.4308</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>175856</v>
+        <v>181548</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>4.7316</v>
+        <v>4.8672</v>
       </c>
       <c r="J11" s="2" t="inlineStr">
         <is>
@@ -4806,19 +4806,19 @@
         </is>
       </c>
       <c r="B12" s="8" t="n">
-        <v>0.005612545969413519</v>
+        <v>0.00286251651171916</v>
       </c>
       <c r="C12" s="2" t="inlineStr"/>
       <c r="D12" s="8" t="n">
-        <v>0.06717707955596475</v>
+        <v>0.0316230266691633</v>
       </c>
       <c r="E12" s="2" t="inlineStr"/>
       <c r="F12" s="8" t="n">
-        <v>0.004229954092545039</v>
+        <v>0.004155435410076765</v>
       </c>
       <c r="G12" s="2" t="inlineStr"/>
       <c r="H12" s="8" t="n">
-        <v>0.006690808421489425</v>
+        <v>0.01693776709446386</v>
       </c>
       <c r="I12" s="2" t="inlineStr"/>
       <c r="J12" s="2" t="inlineStr"/>
@@ -4830,19 +4830,19 @@
         </is>
       </c>
       <c r="B13" s="9" t="n">
-        <v>0.02744212309429701</v>
+        <v>0.020214568040655</v>
       </c>
       <c r="C13" s="2" t="inlineStr"/>
       <c r="D13" s="9" t="n">
-        <v>0.1195118321178747</v>
+        <v>0.1382497395445751</v>
       </c>
       <c r="E13" s="2" t="inlineStr"/>
       <c r="F13" s="9" t="n">
-        <v>0.0062293108636774</v>
+        <v>0.007553415588323804</v>
       </c>
       <c r="G13" s="2" t="inlineStr"/>
       <c r="H13" s="9" t="n">
-        <v>0.1647720025510204</v>
+        <v>0.178265837585034</v>
       </c>
       <c r="I13" s="2" t="inlineStr"/>
       <c r="J13" s="2" t="inlineStr"/>

</xml_diff>